<commit_message>
update to 2 leagues. Working
</commit_message>
<xml_diff>
--- a/goalie_stats.xlsx
+++ b/goalie_stats.xlsx
@@ -4658,7 +4658,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H309"/>
+  <dimension ref="A1:H313"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13652,6 +13652,122 @@
       </c>
       <c r="H309" t="inlineStr"/>
     </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1571842</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Axel Adebrink (20 år)</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>FBC Kalmarsund</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>0</v>
+      </c>
+      <c r="E310" t="n">
+        <v>0</v>
+      </c>
+      <c r="F310" t="n">
+        <v>0</v>
+      </c>
+      <c r="G310" t="inlineStr"/>
+      <c r="H310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1571842</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Pontus Zarins (27 år)</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>FBC Kalmarsund</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>18</v>
+      </c>
+      <c r="E311" t="n">
+        <v>24</v>
+      </c>
+      <c r="F311" t="n">
+        <v>6</v>
+      </c>
+      <c r="G311" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1571842</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Gustav Jansson (34 år)</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>Mullsjö AIS</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>28</v>
+      </c>
+      <c r="E312" t="n">
+        <v>36</v>
+      </c>
+      <c r="F312" t="n">
+        <v>8</v>
+      </c>
+      <c r="G312" t="n">
+        <v>0.778</v>
+      </c>
+      <c r="H312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1571842</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Samuel Jönsson Dolke (20 år)</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Mullsjö AIS</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>0</v>
+      </c>
+      <c r="E313" t="n">
+        <v>0</v>
+      </c>
+      <c r="F313" t="n">
+        <v>0</v>
+      </c>
+      <c r="G313" t="inlineStr"/>
+      <c r="H313" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added game_log and link to each game
</commit_message>
<xml_diff>
--- a/goalie_stats.xlsx
+++ b/goalie_stats.xlsx
@@ -17,7 +17,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -472,7 +476,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571763</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" s="2" t="n">
+        <v>45920.75</v>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -495,7 +501,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571764</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" s="2" t="n">
+        <v>45920.75</v>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -518,7 +526,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571765</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" s="2" t="n">
+        <v>45920.58333333334</v>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -541,7 +551,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571766</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" s="2" t="n">
+        <v>45920.71319444444</v>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -564,7 +576,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571767</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" s="2" t="n">
+        <v>45920.625</v>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -587,7 +601,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571768</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" s="2" t="n">
+        <v>45920.66666666666</v>
+      </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -610,7 +626,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571769</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" s="2" t="n">
+        <v>45920.66666666666</v>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -633,7 +651,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571770</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" s="2" t="n">
+        <v>45923.77083333334</v>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -656,7 +676,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571771</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" s="2" t="n">
+        <v>45923.79166666666</v>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -679,7 +701,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571772</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" s="2" t="n">
+        <v>45924.79166666666</v>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -702,7 +726,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571773</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" s="2" t="n">
+        <v>45924.77083333334</v>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -725,7 +751,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571774</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" s="2" t="n">
+        <v>45924.77083333334</v>
+      </c>
       <c r="D13" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -748,7 +776,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571775</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" s="2" t="n">
+        <v>45923.77083333334</v>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -771,7 +801,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571776</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" s="2" t="n">
+        <v>45925.79166666666</v>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -794,7 +826,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571777</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" s="2" t="n">
+        <v>45927.625</v>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -817,7 +851,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571778</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" s="2" t="n">
+        <v>45928.6875</v>
+      </c>
       <c r="D17" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -840,7 +876,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571779</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" s="2" t="n">
+        <v>45928.79166666666</v>
+      </c>
       <c r="D18" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -863,7 +901,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571780</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" s="2" t="n">
+        <v>45927.66666666666</v>
+      </c>
       <c r="D19" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -886,7 +926,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571781</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" s="2" t="n">
+        <v>45927.71319444444</v>
+      </c>
       <c r="D20" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -909,7 +951,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571782</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" s="2" t="n">
+        <v>45928.66666666666</v>
+      </c>
       <c r="D21" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -932,7 +976,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571783</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" s="2" t="n">
+        <v>45926.77083333334</v>
+      </c>
       <c r="D22" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -955,7 +1001,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571784</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" s="2" t="n">
+        <v>45934.625</v>
+      </c>
       <c r="D23" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -978,7 +1026,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571785</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
+      <c r="C24" s="2" t="n">
+        <v>45934.66666666666</v>
+      </c>
       <c r="D24" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -1001,7 +1051,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571786</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
+      <c r="C25" s="2" t="n">
+        <v>45933.79166666666</v>
+      </c>
       <c r="D25" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -1024,7 +1076,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571787</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
+      <c r="C26" s="2" t="n">
+        <v>45933.82291666666</v>
+      </c>
       <c r="D26" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -1047,7 +1101,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571788</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" s="2" t="n">
+        <v>45934.67708333334</v>
+      </c>
       <c r="D27" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -1070,7 +1126,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571789</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
+      <c r="C28" s="2" t="n">
+        <v>45935.58333333334</v>
+      </c>
       <c r="D28" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -1093,7 +1151,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571790</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
+      <c r="C29" s="2" t="n">
+        <v>45935.70833333334</v>
+      </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -1116,7 +1176,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571791</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" s="2" t="n">
+        <v>45942.70833333334</v>
+      </c>
       <c r="D30" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -1139,7 +1201,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571792</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
+      <c r="C31" s="2" t="n">
+        <v>45942.66666666666</v>
+      </c>
       <c r="D31" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -1162,7 +1226,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571793</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
+      <c r="C32" s="2" t="n">
+        <v>45941.625</v>
+      </c>
       <c r="D32" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -1185,7 +1251,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571794</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr"/>
+      <c r="C33" s="2" t="n">
+        <v>45941.66666666666</v>
+      </c>
       <c r="D33" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -1208,7 +1276,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571795</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr"/>
+      <c r="C34" s="2" t="n">
+        <v>45941.66666666666</v>
+      </c>
       <c r="D34" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -1231,7 +1301,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571796</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr"/>
+      <c r="C35" s="2" t="n">
+        <v>45941.75</v>
+      </c>
       <c r="D35" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -1254,7 +1326,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571797</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
+      <c r="C36" s="2" t="n">
+        <v>45941.70833333334</v>
+      </c>
       <c r="D36" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -1277,7 +1351,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571798</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr"/>
+      <c r="C37" s="2" t="n">
+        <v>45945.77083333334</v>
+      </c>
       <c r="D37" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -1300,7 +1376,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571799</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr"/>
+      <c r="C38" s="2" t="n">
+        <v>45945.79166666666</v>
+      </c>
       <c r="D38" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -1323,7 +1401,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571800</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr"/>
+      <c r="C39" s="2" t="n">
+        <v>45944.77083333334</v>
+      </c>
       <c r="D39" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -1346,7 +1426,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571801</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr"/>
+      <c r="C40" s="2" t="n">
+        <v>45945.77083333334</v>
+      </c>
       <c r="D40" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -1369,7 +1451,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571802</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr"/>
+      <c r="C41" s="2" t="n">
+        <v>45945.79166666666</v>
+      </c>
       <c r="D41" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -1392,7 +1476,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571803</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr"/>
+      <c r="C42" s="2" t="n">
+        <v>45945.79166666666</v>
+      </c>
       <c r="D42" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -1415,7 +1501,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571804</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr"/>
+      <c r="C43" s="2" t="n">
+        <v>45945.79166666666</v>
+      </c>
       <c r="D43" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -1438,7 +1526,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571805</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr"/>
+      <c r="C44" s="2" t="n">
+        <v>45954.79166666666</v>
+      </c>
       <c r="D44" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -1461,7 +1551,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571806</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr"/>
+      <c r="C45" s="2" t="n">
+        <v>45954.77083333334</v>
+      </c>
       <c r="D45" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -1484,7 +1576,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571807</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr"/>
+      <c r="C46" s="2" t="n">
+        <v>45955.67708333334</v>
+      </c>
       <c r="D46" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -1507,7 +1601,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571808</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
+      <c r="C47" s="2" t="n">
+        <v>45956.6875</v>
+      </c>
       <c r="D47" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -1530,7 +1626,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571809</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr"/>
+      <c r="C48" s="2" t="n">
+        <v>45957.79166666666</v>
+      </c>
       <c r="D48" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -1553,7 +1651,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571810</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr"/>
+      <c r="C49" s="2" t="n">
+        <v>45955.66666666666</v>
+      </c>
       <c r="D49" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -1576,7 +1676,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571811</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr"/>
+      <c r="C50" s="2" t="n">
+        <v>45955.66666666666</v>
+      </c>
       <c r="D50" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -1599,7 +1701,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571812</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
+      <c r="C51" s="2" t="n">
+        <v>45962.625</v>
+      </c>
       <c r="D51" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -1622,7 +1726,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571813</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr"/>
+      <c r="C52" s="2" t="n">
+        <v>45961.77083333334</v>
+      </c>
       <c r="D52" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -1645,7 +1751,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571814</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr"/>
+      <c r="C53" s="2" t="n">
+        <v>45961.85416666666</v>
+      </c>
       <c r="D53" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -1668,7 +1776,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571815</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr"/>
+      <c r="C54" s="2" t="n">
+        <v>45962.71319444444</v>
+      </c>
       <c r="D54" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -1691,7 +1801,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571816</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr"/>
+      <c r="C55" s="2" t="n">
+        <v>45963.66666666666</v>
+      </c>
       <c r="D55" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -1714,7 +1826,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571817</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr"/>
+      <c r="C56" s="2" t="n">
+        <v>45963.66666666666</v>
+      </c>
       <c r="D56" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -1737,7 +1851,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571818</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
+      <c r="C57" s="2" t="n">
+        <v>45963.54166666666</v>
+      </c>
       <c r="D57" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -1760,7 +1876,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571819</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr"/>
+      <c r="C58" s="2" t="n">
+        <v>45976.66666666666</v>
+      </c>
       <c r="D58" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -1783,7 +1901,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571820</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr"/>
+      <c r="C59" s="2" t="n">
+        <v>45975.79166666666</v>
+      </c>
       <c r="D59" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -1806,7 +1926,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571821</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr"/>
+      <c r="C60" s="2" t="n">
+        <v>45976.70833333334</v>
+      </c>
       <c r="D60" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -1829,7 +1951,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571822</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr"/>
+      <c r="C61" s="2" t="n">
+        <v>45976.66666666666</v>
+      </c>
       <c r="D61" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -1852,7 +1976,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571823</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr"/>
+      <c r="C62" s="2" t="n">
+        <v>45976.70833333334</v>
+      </c>
       <c r="D62" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -1875,7 +2001,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571824</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr"/>
+      <c r="C63" s="2" t="n">
+        <v>45975.79166666666</v>
+      </c>
       <c r="D63" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -1898,7 +2026,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571825</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr"/>
+      <c r="C64" s="2" t="n">
+        <v>45976.66666666666</v>
+      </c>
       <c r="D64" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -1921,7 +2051,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571826</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr"/>
+      <c r="C65" s="2" t="n">
+        <v>45982.77083333334</v>
+      </c>
       <c r="D65" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -1944,7 +2076,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571827</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr"/>
+      <c r="C66" s="2" t="n">
+        <v>45983.75</v>
+      </c>
       <c r="D66" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -1967,7 +2101,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571828</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr"/>
+      <c r="C67" s="2" t="n">
+        <v>45983.625</v>
+      </c>
       <c r="D67" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -1990,7 +2126,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571829</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr"/>
+      <c r="C68" s="2" t="n">
+        <v>45982.77083333334</v>
+      </c>
       <c r="D68" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -2013,7 +2151,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571830</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr"/>
+      <c r="C69" s="2" t="n">
+        <v>45983.625</v>
+      </c>
       <c r="D69" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -2036,7 +2176,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571831</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr"/>
+      <c r="C70" s="2" t="n">
+        <v>45983.66666666666</v>
+      </c>
       <c r="D70" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -2059,7 +2201,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571832</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr"/>
+      <c r="C71" s="2" t="n">
+        <v>45983.625</v>
+      </c>
       <c r="D71" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -2082,7 +2226,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571833</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr"/>
+      <c r="C72" s="2" t="n">
+        <v>45989.77083333334</v>
+      </c>
       <c r="D72" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -2105,7 +2251,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571834</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr"/>
+      <c r="C73" s="2" t="n">
+        <v>45991.71319444444</v>
+      </c>
       <c r="D73" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -2128,7 +2276,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571835</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr"/>
+      <c r="C74" s="2" t="n">
+        <v>45991.66666666666</v>
+      </c>
       <c r="D74" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -2151,7 +2301,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571836</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr"/>
+      <c r="C75" s="2" t="n">
+        <v>45991.66666666666</v>
+      </c>
       <c r="D75" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -2174,7 +2326,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571837</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
+      <c r="C76" s="2" t="n">
+        <v>45990.75</v>
+      </c>
       <c r="D76" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -2197,7 +2351,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571838</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr"/>
+      <c r="C77" s="2" t="n">
+        <v>45990.70833333334</v>
+      </c>
       <c r="D77" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -2220,7 +2376,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571839</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr"/>
+      <c r="C78" s="2" t="n">
+        <v>45990.66666666666</v>
+      </c>
       <c r="D78" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -2243,7 +2401,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571840</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr"/>
+      <c r="C79" s="2" t="n">
+        <v>45996.82291666666</v>
+      </c>
       <c r="D79" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -2266,7 +2426,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571841</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr"/>
+      <c r="C80" s="2" t="n">
+        <v>45997.625</v>
+      </c>
       <c r="D80" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -2289,7 +2451,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571842</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr"/>
+      <c r="C81" s="2" t="n">
+        <v>45995.79166666666</v>
+      </c>
       <c r="D81" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -2312,7 +2476,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571843</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr"/>
+      <c r="C82" s="2" t="n">
+        <v>45997.66666666666</v>
+      </c>
       <c r="D82" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -2335,7 +2501,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571844</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr"/>
+      <c r="C83" s="2" t="n">
+        <v>45999.79166666666</v>
+      </c>
       <c r="D83" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -2358,7 +2526,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571845</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr"/>
+      <c r="C84" s="2" t="n">
+        <v>45998.66666666666</v>
+      </c>
       <c r="D84" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -2381,7 +2551,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571846</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr"/>
+      <c r="C85" s="2" t="n">
+        <v>45997.70833333334</v>
+      </c>
       <c r="D85" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -2404,7 +2576,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571847</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
+      <c r="C86" s="2" t="n">
+        <v>46011.625</v>
+      </c>
       <c r="D86" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -2427,7 +2601,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571848</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr"/>
+      <c r="C87" s="2" t="n">
+        <v>46011.66666666666</v>
+      </c>
       <c r="D87" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -2450,7 +2626,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571849</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr"/>
+      <c r="C88" s="2" t="n">
+        <v>46011.71319444444</v>
+      </c>
       <c r="D88" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -2473,7 +2651,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571850</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr"/>
+      <c r="C89" s="2" t="n">
+        <v>46011.66666666666</v>
+      </c>
       <c r="D89" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -2496,7 +2676,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571851</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr"/>
+      <c r="C90" s="2" t="n">
+        <v>46011.5625</v>
+      </c>
       <c r="D90" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -2519,7 +2701,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571852</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr"/>
+      <c r="C91" s="2" t="n">
+        <v>46011.66666666666</v>
+      </c>
       <c r="D91" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -2542,7 +2726,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571853</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr"/>
+      <c r="C92" s="2" t="n">
+        <v>46010.79166666666</v>
+      </c>
       <c r="D92" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -2565,7 +2751,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571854</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr"/>
+      <c r="C93" s="2" t="n">
+        <v>46018.70833333334</v>
+      </c>
       <c r="D93" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -2588,7 +2776,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571855</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr"/>
+      <c r="C94" s="2" t="n">
+        <v>46017.66666666666</v>
+      </c>
       <c r="D94" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -2611,7 +2801,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571856</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr"/>
+      <c r="C95" s="2" t="n">
+        <v>46017.66666666666</v>
+      </c>
       <c r="D95" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -2634,7 +2826,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571857</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr"/>
+      <c r="C96" s="2" t="n">
+        <v>46018.625</v>
+      </c>
       <c r="D96" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -2657,7 +2851,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571858</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr"/>
+      <c r="C97" s="2" t="n">
+        <v>46017.77083333334</v>
+      </c>
       <c r="D97" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -2680,7 +2876,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571859</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr"/>
+      <c r="C98" s="2" t="n">
+        <v>46018.70833333334</v>
+      </c>
       <c r="D98" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -2703,7 +2901,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571860</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr"/>
+      <c r="C99" s="2" t="n">
+        <v>46018.66666666666</v>
+      </c>
       <c r="D99" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -2726,7 +2926,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571861</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr"/>
+      <c r="C100" s="2" t="n">
+        <v>46025.625</v>
+      </c>
       <c r="D100" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -2749,7 +2951,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571862</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr"/>
+      <c r="C101" s="2" t="n">
+        <v>46025.66666666666</v>
+      </c>
       <c r="D101" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -2772,7 +2976,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571863</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr"/>
+      <c r="C102" s="2" t="n">
+        <v>46025.83333333334</v>
+      </c>
       <c r="D102" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -2795,7 +3001,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571864</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr"/>
+      <c r="C103" s="2" t="n">
+        <v>46027.79166666666</v>
+      </c>
       <c r="D103" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -2818,7 +3026,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571865</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr"/>
+      <c r="C104" s="2" t="n">
+        <v>46028.67152777778</v>
+      </c>
       <c r="D104" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -2841,7 +3051,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571866</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr"/>
+      <c r="C105" s="2" t="n">
+        <v>46025.52083333334</v>
+      </c>
       <c r="D105" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -2864,7 +3076,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571867</t>
         </is>
       </c>
-      <c r="C106" t="inlineStr"/>
+      <c r="C106" s="2" t="n">
+        <v>46027.75</v>
+      </c>
       <c r="D106" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -2887,7 +3101,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571868</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr"/>
+      <c r="C107" s="2" t="n">
+        <v>46032.625</v>
+      </c>
       <c r="D107" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -2910,7 +3126,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571869</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr"/>
+      <c r="C108" s="2" t="n">
+        <v>46032.66666666666</v>
+      </c>
       <c r="D108" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -2933,7 +3151,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571870</t>
         </is>
       </c>
-      <c r="C109" t="inlineStr"/>
+      <c r="C109" s="2" t="n">
+        <v>46032.75</v>
+      </c>
       <c r="D109" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -2956,7 +3176,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571871</t>
         </is>
       </c>
-      <c r="C110" t="inlineStr"/>
+      <c r="C110" s="2" t="n">
+        <v>46032.6875</v>
+      </c>
       <c r="D110" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -2979,7 +3201,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571872</t>
         </is>
       </c>
-      <c r="C111" t="inlineStr"/>
+      <c r="C111" s="2" t="n">
+        <v>46032.70833333334</v>
+      </c>
       <c r="D111" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -3002,7 +3226,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571873</t>
         </is>
       </c>
-      <c r="C112" t="inlineStr"/>
+      <c r="C112" s="2" t="n">
+        <v>46033.66666666666</v>
+      </c>
       <c r="D112" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -3025,7 +3251,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571874</t>
         </is>
       </c>
-      <c r="C113" t="inlineStr"/>
+      <c r="C113" s="2" t="n">
+        <v>46032.625</v>
+      </c>
       <c r="D113" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -3048,7 +3276,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571875</t>
         </is>
       </c>
-      <c r="C114" t="inlineStr"/>
+      <c r="C114" s="2" t="n">
+        <v>46039.75</v>
+      </c>
       <c r="D114" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -3071,7 +3301,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571876</t>
         </is>
       </c>
-      <c r="C115" t="inlineStr"/>
+      <c r="C115" s="2" t="n">
+        <v>46040.66666666666</v>
+      </c>
       <c r="D115" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -3094,7 +3326,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571877</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr"/>
+      <c r="C116" s="2" t="n">
+        <v>46040.66666666666</v>
+      </c>
       <c r="D116" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -3117,7 +3351,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571878</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr"/>
+      <c r="C117" s="2" t="n">
+        <v>46038.79166666666</v>
+      </c>
       <c r="D117" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -3140,7 +3376,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571879</t>
         </is>
       </c>
-      <c r="C118" t="inlineStr"/>
+      <c r="C118" s="2" t="n">
+        <v>46039.70833333334</v>
+      </c>
       <c r="D118" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -3163,7 +3401,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571880</t>
         </is>
       </c>
-      <c r="C119" t="inlineStr"/>
+      <c r="C119" s="2" t="n">
+        <v>46039.625</v>
+      </c>
       <c r="D119" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -3186,7 +3426,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571881</t>
         </is>
       </c>
-      <c r="C120" t="inlineStr"/>
+      <c r="C120" s="2" t="n">
+        <v>46039.71319444444</v>
+      </c>
       <c r="D120" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -3209,7 +3451,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571882</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr"/>
+      <c r="C121" s="2" t="n">
+        <v>46046.625</v>
+      </c>
       <c r="D121" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -3232,7 +3476,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571883</t>
         </is>
       </c>
-      <c r="C122" t="inlineStr"/>
+      <c r="C122" s="2" t="n">
+        <v>46046.6875</v>
+      </c>
       <c r="D122" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -3255,7 +3501,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571884</t>
         </is>
       </c>
-      <c r="C123" t="inlineStr"/>
+      <c r="C123" s="2" t="n">
+        <v>46046.625</v>
+      </c>
       <c r="D123" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -3278,7 +3526,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571885</t>
         </is>
       </c>
-      <c r="C124" t="inlineStr"/>
+      <c r="C124" s="2" t="n">
+        <v>46064.77083333334</v>
+      </c>
       <c r="D124" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -3301,7 +3551,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571886</t>
         </is>
       </c>
-      <c r="C125" t="inlineStr"/>
+      <c r="C125" s="2" t="n">
+        <v>46046.625</v>
+      </c>
       <c r="D125" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -3324,7 +3576,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571887</t>
         </is>
       </c>
-      <c r="C126" t="inlineStr"/>
+      <c r="C126" s="2" t="n">
+        <v>46046.66666666666</v>
+      </c>
       <c r="D126" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -3347,7 +3601,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571888</t>
         </is>
       </c>
-      <c r="C127" t="inlineStr"/>
+      <c r="C127" s="2" t="n">
+        <v>46046.66666666666</v>
+      </c>
       <c r="D127" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -3370,7 +3626,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571889</t>
         </is>
       </c>
-      <c r="C128" t="inlineStr"/>
+      <c r="C128" s="2" t="n">
+        <v>46050.77083333334</v>
+      </c>
       <c r="D128" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -3393,7 +3651,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571890</t>
         </is>
       </c>
-      <c r="C129" t="inlineStr"/>
+      <c r="C129" s="2" t="n">
+        <v>46049.79166666666</v>
+      </c>
       <c r="D129" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -3416,7 +3676,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571891</t>
         </is>
       </c>
-      <c r="C130" t="inlineStr"/>
+      <c r="C130" s="2" t="n">
+        <v>46050.77083333334</v>
+      </c>
       <c r="D130" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -3439,7 +3701,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571892</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr"/>
+      <c r="C131" s="2" t="n">
+        <v>46049.77083333334</v>
+      </c>
       <c r="D131" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -3462,7 +3726,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571893</t>
         </is>
       </c>
-      <c r="C132" t="inlineStr"/>
+      <c r="C132" s="2" t="n">
+        <v>46050.77083333334</v>
+      </c>
       <c r="D132" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -3485,7 +3751,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571894</t>
         </is>
       </c>
-      <c r="C133" t="inlineStr"/>
+      <c r="C133" s="2" t="n">
+        <v>46050.79166666666</v>
+      </c>
       <c r="D133" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -3508,7 +3776,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571895</t>
         </is>
       </c>
-      <c r="C134" t="inlineStr"/>
+      <c r="C134" s="2" t="n">
+        <v>46050.77083333334</v>
+      </c>
       <c r="D134" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -3531,7 +3801,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571896</t>
         </is>
       </c>
-      <c r="C135" t="inlineStr"/>
+      <c r="C135" s="2" t="n">
+        <v>46052.77083333334</v>
+      </c>
       <c r="D135" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -3554,7 +3826,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571897</t>
         </is>
       </c>
-      <c r="C136" t="inlineStr"/>
+      <c r="C136" s="2" t="n">
+        <v>46053.75</v>
+      </c>
       <c r="D136" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -3577,7 +3851,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571898</t>
         </is>
       </c>
-      <c r="C137" t="inlineStr"/>
+      <c r="C137" s="2" t="n">
+        <v>46054.54166666666</v>
+      </c>
       <c r="D137" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -3600,7 +3876,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571899</t>
         </is>
       </c>
-      <c r="C138" t="inlineStr"/>
+      <c r="C138" s="2" t="n">
+        <v>46053.625</v>
+      </c>
       <c r="D138" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -3623,7 +3901,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571900</t>
         </is>
       </c>
-      <c r="C139" t="inlineStr"/>
+      <c r="C139" s="2" t="n">
+        <v>46052.77083333334</v>
+      </c>
       <c r="D139" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -3646,7 +3926,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571901</t>
         </is>
       </c>
-      <c r="C140" t="inlineStr"/>
+      <c r="C140" s="2" t="n">
+        <v>46053.71319444444</v>
+      </c>
       <c r="D140" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -3669,7 +3951,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571902</t>
         </is>
       </c>
-      <c r="C141" t="inlineStr"/>
+      <c r="C141" s="2" t="n">
+        <v>46053.625</v>
+      </c>
       <c r="D141" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -3692,7 +3976,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571903</t>
         </is>
       </c>
-      <c r="C142" t="inlineStr"/>
+      <c r="C142" s="2" t="n">
+        <v>46067.60416666666</v>
+      </c>
       <c r="D142" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -3715,7 +4001,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571904</t>
         </is>
       </c>
-      <c r="C143" t="inlineStr"/>
+      <c r="C143" s="2" t="n">
+        <v>46068.66666666666</v>
+      </c>
       <c r="D143" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -3738,7 +4026,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571905</t>
         </is>
       </c>
-      <c r="C144" t="inlineStr"/>
+      <c r="C144" s="2" t="n">
+        <v>46067.70833333334</v>
+      </c>
       <c r="D144" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -3761,7 +4051,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571906</t>
         </is>
       </c>
-      <c r="C145" t="inlineStr"/>
+      <c r="C145" s="2" t="n">
+        <v>46068.6875</v>
+      </c>
       <c r="D145" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -3784,7 +4076,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571907</t>
         </is>
       </c>
-      <c r="C146" t="inlineStr"/>
+      <c r="C146" s="2" t="n">
+        <v>46067.625</v>
+      </c>
       <c r="D146" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -3807,7 +4101,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571908</t>
         </is>
       </c>
-      <c r="C147" t="inlineStr"/>
+      <c r="C147" s="2" t="n">
+        <v>46067.66666666666</v>
+      </c>
       <c r="D147" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -3830,7 +4126,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571909</t>
         </is>
       </c>
-      <c r="C148" t="inlineStr"/>
+      <c r="C148" s="2" t="n">
+        <v>46067.58333333334</v>
+      </c>
       <c r="D148" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -3853,7 +4151,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571910</t>
         </is>
       </c>
-      <c r="C149" t="inlineStr"/>
+      <c r="C149" s="2" t="n">
+        <v>46075.66666666666</v>
+      </c>
       <c r="D149" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -3876,7 +4176,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571911</t>
         </is>
       </c>
-      <c r="C150" t="inlineStr"/>
+      <c r="C150" s="2" t="n">
+        <v>46073.79166666666</v>
+      </c>
       <c r="D150" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -3899,7 +4201,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571912</t>
         </is>
       </c>
-      <c r="C151" t="inlineStr"/>
+      <c r="C151" s="2" t="n">
+        <v>46074.625</v>
+      </c>
       <c r="D151" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -3922,7 +4226,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571913</t>
         </is>
       </c>
-      <c r="C152" t="inlineStr"/>
+      <c r="C152" s="2" t="n">
+        <v>46074.66666666666</v>
+      </c>
       <c r="D152" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -3945,7 +4251,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571914</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr"/>
+      <c r="C153" s="2" t="n">
+        <v>46075.66666666666</v>
+      </c>
       <c r="D153" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -3968,7 +4276,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571915</t>
         </is>
       </c>
-      <c r="C154" t="inlineStr"/>
+      <c r="C154" s="2" t="n">
+        <v>46073.79166666666</v>
+      </c>
       <c r="D154" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -3991,7 +4301,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571916</t>
         </is>
       </c>
-      <c r="C155" t="inlineStr"/>
+      <c r="C155" s="2" t="n">
+        <v>46074.71319444444</v>
+      </c>
       <c r="D155" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -4014,7 +4326,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571917</t>
         </is>
       </c>
-      <c r="C156" t="inlineStr"/>
+      <c r="C156" s="2" t="n">
+        <v>46080.77083333334</v>
+      </c>
       <c r="D156" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -4037,7 +4351,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571918</t>
         </is>
       </c>
-      <c r="C157" t="inlineStr"/>
+      <c r="C157" s="2" t="n">
+        <v>46082.66666666666</v>
+      </c>
       <c r="D157" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -4060,7 +4376,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571919</t>
         </is>
       </c>
-      <c r="C158" t="inlineStr"/>
+      <c r="C158" s="2" t="n">
+        <v>46081.70833333334</v>
+      </c>
       <c r="D158" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -4083,7 +4401,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571920</t>
         </is>
       </c>
-      <c r="C159" t="inlineStr"/>
+      <c r="C159" s="2" t="n">
+        <v>46081.71319444444</v>
+      </c>
       <c r="D159" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -4106,7 +4426,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571921</t>
         </is>
       </c>
-      <c r="C160" t="inlineStr"/>
+      <c r="C160" s="2" t="n">
+        <v>46081.6875</v>
+      </c>
       <c r="D160" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -4129,7 +4451,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571922</t>
         </is>
       </c>
-      <c r="C161" t="inlineStr"/>
+      <c r="C161" s="2" t="n">
+        <v>46081.625</v>
+      </c>
       <c r="D161" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -4152,7 +4476,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571923</t>
         </is>
       </c>
-      <c r="C162" t="inlineStr"/>
+      <c r="C162" s="2" t="n">
+        <v>46081.66666666666</v>
+      </c>
       <c r="D162" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -4175,7 +4501,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571924</t>
         </is>
       </c>
-      <c r="C163" t="inlineStr"/>
+      <c r="C163" s="2" t="n">
+        <v>46084.77083333334</v>
+      </c>
       <c r="D163" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -4198,7 +4526,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571925</t>
         </is>
       </c>
-      <c r="C164" t="inlineStr"/>
+      <c r="C164" s="2" t="n">
+        <v>46085.79166666666</v>
+      </c>
       <c r="D164" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -4221,7 +4551,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571926</t>
         </is>
       </c>
-      <c r="C165" t="inlineStr"/>
+      <c r="C165" s="2" t="n">
+        <v>46086.77083333334</v>
+      </c>
       <c r="D165" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -4244,7 +4576,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571927</t>
         </is>
       </c>
-      <c r="C166" t="inlineStr"/>
+      <c r="C166" s="2" t="n">
+        <v>46085.79166666666</v>
+      </c>
       <c r="D166" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -4267,7 +4601,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571928</t>
         </is>
       </c>
-      <c r="C167" t="inlineStr"/>
+      <c r="C167" s="2" t="n">
+        <v>46085.79166666666</v>
+      </c>
       <c r="D167" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -4290,7 +4626,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571929</t>
         </is>
       </c>
-      <c r="C168" t="inlineStr"/>
+      <c r="C168" s="2" t="n">
+        <v>46085.79166666666</v>
+      </c>
       <c r="D168" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -4313,7 +4651,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571930</t>
         </is>
       </c>
-      <c r="C169" t="inlineStr"/>
+      <c r="C169" s="2" t="n">
+        <v>46085.79166666666</v>
+      </c>
       <c r="D169" t="inlineStr">
         <is>
           <t>Nykvarns IBF</t>
@@ -4336,7 +4676,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571931</t>
         </is>
       </c>
-      <c r="C170" t="inlineStr"/>
+      <c r="C170" s="2" t="n">
+        <v>46087.79166666666</v>
+      </c>
       <c r="D170" t="inlineStr">
         <is>
           <t>Pixbo IBK</t>
@@ -4359,7 +4701,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571932</t>
         </is>
       </c>
-      <c r="C171" t="inlineStr"/>
+      <c r="C171" s="2" t="n">
+        <v>46088.71319444444</v>
+      </c>
       <c r="D171" t="inlineStr">
         <is>
           <t>IBF Falun</t>
@@ -4382,7 +4726,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571933</t>
         </is>
       </c>
-      <c r="C172" t="inlineStr"/>
+      <c r="C172" s="2" t="n">
+        <v>46088.66666666666</v>
+      </c>
       <c r="D172" t="inlineStr">
         <is>
           <t>Mullsjö AIS</t>
@@ -4405,7 +4751,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571934</t>
         </is>
       </c>
-      <c r="C173" t="inlineStr"/>
+      <c r="C173" s="2" t="n">
+        <v>46089.6875</v>
+      </c>
       <c r="D173" t="inlineStr">
         <is>
           <t>Hovslätts IK</t>
@@ -4428,7 +4776,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571935</t>
         </is>
       </c>
-      <c r="C174" t="inlineStr"/>
+      <c r="C174" s="2" t="n">
+        <v>46088.625</v>
+      </c>
       <c r="D174" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -4451,7 +4801,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571936</t>
         </is>
       </c>
-      <c r="C175" t="inlineStr"/>
+      <c r="C175" s="2" t="n">
+        <v>46088.625</v>
+      </c>
       <c r="D175" t="inlineStr">
         <is>
           <t>Warberg IC</t>
@@ -4474,7 +4826,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571937</t>
         </is>
       </c>
-      <c r="C176" t="inlineStr"/>
+      <c r="C176" s="2" t="n">
+        <v>46089.625</v>
+      </c>
       <c r="D176" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
@@ -4497,7 +4851,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571938</t>
         </is>
       </c>
-      <c r="C177" t="inlineStr"/>
+      <c r="C177" s="2" t="n">
+        <v>46095.66666666666</v>
+      </c>
       <c r="D177" t="inlineStr">
         <is>
           <t>Storvreta IBK</t>
@@ -4520,7 +4876,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571939</t>
         </is>
       </c>
-      <c r="C178" t="inlineStr"/>
+      <c r="C178" s="2" t="n">
+        <v>46095.66666666666</v>
+      </c>
       <c r="D178" t="inlineStr">
         <is>
           <t>Visby IBK</t>
@@ -4543,7 +4901,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571940</t>
         </is>
       </c>
-      <c r="C179" t="inlineStr"/>
+      <c r="C179" s="2" t="n">
+        <v>46095.66666666666</v>
+      </c>
       <c r="D179" t="inlineStr">
         <is>
           <t>FBC Kalmarsund</t>
@@ -4566,7 +4926,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571941</t>
         </is>
       </c>
-      <c r="C180" t="inlineStr"/>
+      <c r="C180" s="2" t="n">
+        <v>46095.66666666666</v>
+      </c>
       <c r="D180" t="inlineStr">
         <is>
           <t>Strängnäs IBK</t>
@@ -4589,7 +4951,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571942</t>
         </is>
       </c>
-      <c r="C181" t="inlineStr"/>
+      <c r="C181" s="2" t="n">
+        <v>46095.66666666666</v>
+      </c>
       <c r="D181" t="inlineStr">
         <is>
           <t>AIK IBF</t>
@@ -4612,7 +4976,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571943</t>
         </is>
       </c>
-      <c r="C182" t="inlineStr"/>
+      <c r="C182" s="2" t="n">
+        <v>46095.66666666666</v>
+      </c>
       <c r="D182" t="inlineStr">
         <is>
           <t>Linköping IBK</t>
@@ -4635,7 +5001,9 @@
           <t>http://statistik.innebandy.se/ft.aspx?scr=result&amp;fmid=1571944</t>
         </is>
       </c>
-      <c r="C183" t="inlineStr"/>
+      <c r="C183" s="2" t="n">
+        <v>46095.66666666666</v>
+      </c>
       <c r="D183" t="inlineStr">
         <is>
           <t>Jönköpings IK</t>
@@ -4658,7 +5026,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H333"/>
+  <dimension ref="A1:H337"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14121,17 +14489,17 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>1571845</t>
+          <t>1571844</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Emil Lindblom (23 år)</t>
+          <t>Oskar Bäckman (19 år)</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>Storvreta IBK</t>
+          <t>AIK IBF</t>
         </is>
       </c>
       <c r="D326" t="n">
@@ -14149,47 +14517,45 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>1571845</t>
+          <t>1571844</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Måns Parsjö (31 år)</t>
+          <t>Jonathan Hjelm (27 år)</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>Storvreta IBK</t>
+          <t>AIK IBF</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E327" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F327" t="n">
-        <v>3</v>
-      </c>
-      <c r="G327" t="n">
-        <v>0.667</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G327" t="inlineStr"/>
       <c r="H327" t="inlineStr"/>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>1571845</t>
+          <t>1571844</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Olle Jonsson (25 år)</t>
+          <t>Wiktor Åkerstedt (30 år)</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>Warberg IC</t>
+          <t>Strängnäs IBK</t>
         </is>
       </c>
       <c r="D328" t="n">
@@ -14207,148 +14573,262 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>1571845</t>
+          <t>1571844</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Nicholay Halvorsen (25 år)</t>
+          <t>Oskar-Viking Tjärnberg (28 år)</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>Warberg IC</t>
+          <t>Strängnäs IBK</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E329" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F329" t="n">
-        <v>5</v>
-      </c>
-      <c r="G329" t="n">
-        <v>0.615</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G329" t="inlineStr"/>
       <c r="H329" t="inlineStr"/>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>1571846</t>
+          <t>1571845</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Rasmus Ekström (30 år)</t>
+          <t>Emil Lindblom (23 år)</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>Visby IBK</t>
+          <t>Storvreta IBK</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="E330" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="F330" t="n">
-        <v>11</v>
-      </c>
-      <c r="G330" t="n">
-        <v>0.711</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G330" t="inlineStr"/>
       <c r="H330" t="inlineStr"/>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>1571846</t>
+          <t>1571845</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Andreas Egegård (28 år)</t>
+          <t>Måns Parsjö (31 år)</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>Visby IBK</t>
+          <t>Storvreta IBK</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E331" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F331" t="n">
-        <v>0</v>
-      </c>
-      <c r="G331" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="G331" t="n">
+        <v>0.667</v>
+      </c>
       <c r="H331" t="inlineStr"/>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>1571846</t>
+          <t>1571845</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>Santtu Strandberg (34 år)</t>
+          <t>Olle Jonsson (25 år)</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>Växjö IBK</t>
+          <t>Warberg IC</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E332" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F332" t="n">
-        <v>10</v>
-      </c>
-      <c r="G332" t="n">
-        <v>0.63</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G332" t="inlineStr"/>
       <c r="H332" t="inlineStr"/>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
+          <t>1571845</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Nicholay Halvorsen (25 år)</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>Warberg IC</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>8</v>
+      </c>
+      <c r="E333" t="n">
+        <v>13</v>
+      </c>
+      <c r="F333" t="n">
+        <v>5</v>
+      </c>
+      <c r="G333" t="n">
+        <v>0.615</v>
+      </c>
+      <c r="H333" t="inlineStr"/>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
           <t>1571846</t>
         </is>
       </c>
-      <c r="B333" t="inlineStr">
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Rasmus Ekström (30 år)</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>Visby IBK</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>27</v>
+      </c>
+      <c r="E334" t="n">
+        <v>38</v>
+      </c>
+      <c r="F334" t="n">
+        <v>11</v>
+      </c>
+      <c r="G334" t="n">
+        <v>0.711</v>
+      </c>
+      <c r="H334" t="inlineStr"/>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1571846</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Andreas Egegård (28 år)</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>Visby IBK</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>0</v>
+      </c>
+      <c r="E335" t="n">
+        <v>0</v>
+      </c>
+      <c r="F335" t="n">
+        <v>0</v>
+      </c>
+      <c r="G335" t="inlineStr"/>
+      <c r="H335" t="inlineStr"/>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1571846</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Santtu Strandberg (34 år)</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>Växjö IBK</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>17</v>
+      </c>
+      <c r="E336" t="n">
+        <v>27</v>
+      </c>
+      <c r="F336" t="n">
+        <v>10</v>
+      </c>
+      <c r="G336" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="H336" t="inlineStr"/>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1571846</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
         <is>
           <t>Noel Johansson (19 år)</t>
         </is>
       </c>
-      <c r="C333" t="inlineStr">
+      <c r="C337" t="inlineStr">
         <is>
           <t>Växjö IBK</t>
         </is>
       </c>
-      <c r="D333" t="n">
-        <v>0</v>
-      </c>
-      <c r="E333" t="n">
-        <v>0</v>
-      </c>
-      <c r="F333" t="n">
-        <v>0</v>
-      </c>
-      <c r="G333" t="inlineStr"/>
-      <c r="H333" t="inlineStr"/>
+      <c r="D337" t="n">
+        <v>0</v>
+      </c>
+      <c r="E337" t="n">
+        <v>0</v>
+      </c>
+      <c r="F337" t="n">
+        <v>0</v>
+      </c>
+      <c r="G337" t="inlineStr"/>
+      <c r="H337" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fetches data even if not in table
</commit_message>
<xml_diff>
--- a/goalie_stats.xlsx
+++ b/goalie_stats.xlsx
@@ -14531,15 +14531,17 @@
         </is>
       </c>
       <c r="D327" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E327" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F327" t="n">
-        <v>0</v>
-      </c>
-      <c r="G327" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="G327" t="n">
+        <v>0.767</v>
+      </c>
       <c r="H327" t="inlineStr"/>
     </row>
     <row r="328">
@@ -14559,15 +14561,17 @@
         </is>
       </c>
       <c r="D328" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E328" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F328" t="n">
-        <v>0</v>
-      </c>
-      <c r="G328" t="inlineStr"/>
+        <v>6</v>
+      </c>
+      <c r="G328" t="n">
+        <v>0.769</v>
+      </c>
       <c r="H328" t="inlineStr"/>
     </row>
     <row r="329">

</xml_diff>